<commit_message>
de identifying nba players
</commit_message>
<xml_diff>
--- a/NBA Data File.xlsx
+++ b/NBA Data File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YZH79C\Documents\SIADS591_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86914BFB-3DEC-40FB-A086-406B010A2BD3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AF903E-E2F6-48CB-AC9D-84C068C6D025}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="699">
   <si>
     <t>Name</t>
   </si>
@@ -2121,6 +2121,9 @@
   <si>
     <t>Okobo, Elie</t>
   </si>
+  <si>
+    <t>Name(de-identified</t>
+  </si>
 </sst>
 </file>
 
@@ -2220,7 +2223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2267,6 +2270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -45078,19 +45082,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" customWidth="1"/>
     <col min="30" max="30" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:157">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="20" t="s">
+        <v>698</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -45342,8 +45346,8 @@
       <c r="FA1" s="1"/>
     </row>
     <row r="2" spans="1:157" ht="15" thickBot="1">
-      <c r="A2" t="s">
-        <v>245</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -45485,8 +45489,8 @@
       </c>
     </row>
     <row r="3" spans="1:157" ht="15" thickBot="1">
-      <c r="A3" t="s">
-        <v>203</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -45628,8 +45632,8 @@
       </c>
     </row>
     <row r="4" spans="1:157" ht="15" thickBot="1">
-      <c r="A4" t="s">
-        <v>169</v>
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -45771,8 +45775,8 @@
       </c>
     </row>
     <row r="5" spans="1:157" ht="15" thickBot="1">
-      <c r="A5" t="s">
-        <v>54</v>
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -45914,8 +45918,8 @@
       </c>
     </row>
     <row r="6" spans="1:157" ht="15" thickBot="1">
-      <c r="A6" t="s">
-        <v>145</v>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -46054,8 +46058,8 @@
       </c>
     </row>
     <row r="7" spans="1:157">
-      <c r="A7" t="s">
-        <v>637</v>
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -46197,8 +46201,8 @@
       </c>
     </row>
     <row r="8" spans="1:157">
-      <c r="A8" t="s">
-        <v>139</v>
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -46340,8 +46344,8 @@
       </c>
     </row>
     <row r="9" spans="1:157">
-      <c r="A9" t="s">
-        <v>402</v>
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -46483,8 +46487,8 @@
       </c>
     </row>
     <row r="10" spans="1:157" ht="15" thickBot="1">
-      <c r="A10" t="s">
-        <v>277</v>
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -46626,8 +46630,8 @@
       </c>
     </row>
     <row r="11" spans="1:157" ht="15" thickBot="1">
-      <c r="A11" t="s">
-        <v>558</v>
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -46763,8 +46767,8 @@
       </c>
     </row>
     <row r="12" spans="1:157" ht="15" thickBot="1">
-      <c r="A12" t="s">
-        <v>337</v>
+      <c r="A12">
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -46906,8 +46910,8 @@
       </c>
     </row>
     <row r="13" spans="1:157" ht="15" thickBot="1">
-      <c r="A13" t="s">
-        <v>358</v>
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -47049,8 +47053,8 @@
       </c>
     </row>
     <row r="14" spans="1:157" ht="15" thickBot="1">
-      <c r="A14" t="s">
-        <v>507</v>
+      <c r="A14">
+        <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
@@ -47192,8 +47196,8 @@
       </c>
     </row>
     <row r="15" spans="1:157">
-      <c r="A15" t="s">
-        <v>530</v>
+      <c r="A15">
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -47335,8 +47339,8 @@
       </c>
     </row>
     <row r="16" spans="1:157">
-      <c r="A16" t="s">
-        <v>99</v>
+      <c r="A16">
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -47478,8 +47482,8 @@
       </c>
     </row>
     <row r="17" spans="1:47">
-      <c r="A17" t="s">
-        <v>400</v>
+      <c r="A17">
+        <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -47621,8 +47625,8 @@
       </c>
     </row>
     <row r="18" spans="1:47" ht="15" thickBot="1">
-      <c r="A18" t="s">
-        <v>656</v>
+      <c r="A18">
+        <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -47764,8 +47768,8 @@
       </c>
     </row>
     <row r="19" spans="1:47">
-      <c r="A19" t="s">
-        <v>328</v>
+      <c r="A19">
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -47907,8 +47911,8 @@
       </c>
     </row>
     <row r="20" spans="1:47" ht="15" thickBot="1">
-      <c r="A20" t="s">
-        <v>612</v>
+      <c r="A20">
+        <v>1</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -48050,8 +48054,8 @@
       </c>
     </row>
     <row r="21" spans="1:47" ht="15" thickBot="1">
-      <c r="A21" t="s">
-        <v>427</v>
+      <c r="A21">
+        <v>1</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
@@ -48193,8 +48197,8 @@
       </c>
     </row>
     <row r="22" spans="1:47">
-      <c r="A22" t="s">
-        <v>141</v>
+      <c r="A22">
+        <v>1</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -48336,8 +48340,8 @@
       </c>
     </row>
     <row r="23" spans="1:47">
-      <c r="A23" t="s">
-        <v>626</v>
+      <c r="A23">
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -48479,8 +48483,8 @@
       </c>
     </row>
     <row r="24" spans="1:47" ht="15" thickBot="1">
-      <c r="A24" t="s">
-        <v>101</v>
+      <c r="A24">
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
@@ -48616,8 +48620,8 @@
       </c>
     </row>
     <row r="25" spans="1:47">
-      <c r="A25" t="s">
-        <v>351</v>
+      <c r="A25">
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
@@ -48756,8 +48760,8 @@
       </c>
     </row>
     <row r="26" spans="1:47" ht="15" thickBot="1">
-      <c r="A26" t="s">
-        <v>522</v>
+      <c r="A26">
+        <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -48896,8 +48900,8 @@
       </c>
     </row>
     <row r="27" spans="1:47">
-      <c r="A27" t="s">
-        <v>394</v>
+      <c r="A27">
+        <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -49039,8 +49043,8 @@
       </c>
     </row>
     <row r="28" spans="1:47">
-      <c r="A28" t="s">
-        <v>545</v>
+      <c r="A28">
+        <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
@@ -49182,8 +49186,8 @@
       </c>
     </row>
     <row r="29" spans="1:47">
-      <c r="A29" t="s">
-        <v>447</v>
+      <c r="A29">
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>21</v>
@@ -49325,8 +49329,8 @@
       </c>
     </row>
     <row r="30" spans="1:47" ht="15" thickBot="1">
-      <c r="A30" t="s">
-        <v>87</v>
+      <c r="A30">
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -49468,8 +49472,8 @@
       </c>
     </row>
     <row r="31" spans="1:47" ht="15" thickBot="1">
-      <c r="A31" t="s">
-        <v>372</v>
+      <c r="A31">
+        <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -49611,8 +49615,8 @@
       </c>
     </row>
     <row r="32" spans="1:47" ht="15" thickBot="1">
-      <c r="A32" t="s">
-        <v>368</v>
+      <c r="A32">
+        <v>1</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -49754,8 +49758,8 @@
       </c>
     </row>
     <row r="33" spans="1:47" ht="15" thickBot="1">
-      <c r="A33" t="s">
-        <v>516</v>
+      <c r="A33">
+        <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
@@ -49897,8 +49901,8 @@
       </c>
     </row>
     <row r="34" spans="1:47" ht="15" thickBot="1">
-      <c r="A34" t="s">
-        <v>24</v>
+      <c r="A34">
+        <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
@@ -50037,8 +50041,8 @@
       </c>
     </row>
     <row r="35" spans="1:47" ht="15" thickBot="1">
-      <c r="A35" t="s">
-        <v>616</v>
+      <c r="A35">
+        <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
@@ -50180,8 +50184,8 @@
       </c>
     </row>
     <row r="36" spans="1:47" ht="15" thickBot="1">
-      <c r="A36" t="s">
-        <v>498</v>
+      <c r="A36">
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>21</v>
@@ -50323,8 +50327,8 @@
       </c>
     </row>
     <row r="37" spans="1:47" ht="15" thickBot="1">
-      <c r="A37" t="s">
-        <v>196</v>
+      <c r="A37">
+        <v>1</v>
       </c>
       <c r="B37" t="s">
         <v>28</v>
@@ -50466,8 +50470,8 @@
       </c>
     </row>
     <row r="38" spans="1:47" ht="15" thickBot="1">
-      <c r="A38" t="s">
-        <v>121</v>
+      <c r="A38">
+        <v>1</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
@@ -50609,8 +50613,8 @@
       </c>
     </row>
     <row r="39" spans="1:47">
-      <c r="A39" t="s">
-        <v>316</v>
+      <c r="A39">
+        <v>1</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
@@ -50752,8 +50756,8 @@
       </c>
     </row>
     <row r="40" spans="1:47" ht="15" thickBot="1">
-      <c r="A40" t="s">
-        <v>489</v>
+      <c r="A40">
+        <v>1</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
@@ -50895,8 +50899,8 @@
       </c>
     </row>
     <row r="41" spans="1:47" ht="15" thickBot="1">
-      <c r="A41" t="s">
-        <v>572</v>
+      <c r="A41">
+        <v>1</v>
       </c>
       <c r="B41" t="s">
         <v>31</v>
@@ -51038,8 +51042,8 @@
       </c>
     </row>
     <row r="42" spans="1:47">
-      <c r="A42" t="s">
-        <v>496</v>
+      <c r="A42">
+        <v>1</v>
       </c>
       <c r="B42" t="s">
         <v>36</v>
@@ -51181,8 +51185,8 @@
       </c>
     </row>
     <row r="43" spans="1:47" ht="15" thickBot="1">
-      <c r="A43" t="s">
-        <v>192</v>
+      <c r="A43">
+        <v>1</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -51324,8 +51328,8 @@
       </c>
     </row>
     <row r="44" spans="1:47" ht="15" thickBot="1">
-      <c r="A44" t="s">
-        <v>52</v>
+      <c r="A44">
+        <v>1</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
@@ -51467,8 +51471,8 @@
       </c>
     </row>
     <row r="45" spans="1:47">
-      <c r="A45" t="s">
-        <v>73</v>
+      <c r="A45">
+        <v>1</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
@@ -51604,8 +51608,8 @@
       </c>
     </row>
     <row r="46" spans="1:47">
-      <c r="A46" t="s">
-        <v>623</v>
+      <c r="A46">
+        <v>1</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
@@ -51747,8 +51751,8 @@
       </c>
     </row>
     <row r="47" spans="1:47" ht="15" thickBot="1">
-      <c r="A47" t="s">
-        <v>378</v>
+      <c r="A47">
+        <v>1</v>
       </c>
       <c r="B47" t="s">
         <v>25</v>
@@ -51890,8 +51894,8 @@
       </c>
     </row>
     <row r="48" spans="1:47" ht="15" thickBot="1">
-      <c r="A48" t="s">
-        <v>183</v>
+      <c r="A48">
+        <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>28</v>
@@ -52033,8 +52037,8 @@
       </c>
     </row>
     <row r="49" spans="1:47">
-      <c r="A49" t="s">
-        <v>553</v>
+      <c r="A49">
+        <v>1</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
@@ -52171,8 +52175,8 @@
       </c>
     </row>
     <row r="50" spans="1:47" ht="15" thickBot="1">
-      <c r="A50" t="s">
-        <v>160</v>
+      <c r="A50">
+        <v>1</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -52314,8 +52318,8 @@
       </c>
     </row>
     <row r="51" spans="1:47">
-      <c r="A51" t="s">
-        <v>63</v>
+      <c r="A51">
+        <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>31</v>
@@ -52457,8 +52461,8 @@
       </c>
     </row>
     <row r="52" spans="1:47">
-      <c r="A52" t="s">
-        <v>251</v>
+      <c r="A52">
+        <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
@@ -52600,8 +52604,8 @@
       </c>
     </row>
     <row r="53" spans="1:47">
-      <c r="A53" t="s">
-        <v>480</v>
+      <c r="A53">
+        <v>1</v>
       </c>
       <c r="B53" t="s">
         <v>21</v>
@@ -52743,8 +52747,8 @@
       </c>
     </row>
     <row r="54" spans="1:47">
-      <c r="A54" t="s">
-        <v>243</v>
+      <c r="A54">
+        <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
@@ -52886,8 +52890,8 @@
       </c>
     </row>
     <row r="55" spans="1:47" ht="15" thickBot="1">
-      <c r="A55" t="s">
-        <v>382</v>
+      <c r="A55">
+        <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>31</v>
@@ -53029,8 +53033,8 @@
       </c>
     </row>
     <row r="56" spans="1:47" ht="15" thickBot="1">
-      <c r="A56" t="s">
-        <v>155</v>
+      <c r="A56">
+        <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>25</v>
@@ -53172,8 +53176,8 @@
       </c>
     </row>
     <row r="57" spans="1:47" ht="15" thickBot="1">
-      <c r="A57" t="s">
-        <v>33</v>
+      <c r="A57">
+        <v>1</v>
       </c>
       <c r="B57" t="s">
         <v>31</v>
@@ -53315,8 +53319,8 @@
       </c>
     </row>
     <row r="58" spans="1:47" ht="15" thickBot="1">
-      <c r="A58" t="s">
-        <v>225</v>
+      <c r="A58">
+        <v>1</v>
       </c>
       <c r="B58" t="s">
         <v>31</v>
@@ -53458,8 +53462,8 @@
       </c>
     </row>
     <row r="59" spans="1:47" ht="15" thickBot="1">
-      <c r="A59" t="s">
-        <v>642</v>
+      <c r="A59">
+        <v>1</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -53601,8 +53605,8 @@
       </c>
     </row>
     <row r="60" spans="1:47" ht="15" thickBot="1">
-      <c r="A60" t="s">
-        <v>308</v>
+      <c r="A60">
+        <v>1</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -53729,8 +53733,8 @@
       </c>
     </row>
     <row r="61" spans="1:47" ht="15" thickBot="1">
-      <c r="A61" t="s">
-        <v>35</v>
+      <c r="A61">
+        <v>1</v>
       </c>
       <c r="B61" t="s">
         <v>36</v>
@@ -53872,8 +53876,8 @@
       </c>
     </row>
     <row r="62" spans="1:47" ht="15" thickBot="1">
-      <c r="A62" t="s">
-        <v>535</v>
+      <c r="A62">
+        <v>1</v>
       </c>
       <c r="B62" t="s">
         <v>31</v>
@@ -54009,8 +54013,8 @@
       </c>
     </row>
     <row r="63" spans="1:47" ht="15" thickBot="1">
-      <c r="A63" t="s">
-        <v>520</v>
+      <c r="A63">
+        <v>1</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
@@ -54143,8 +54147,8 @@
       </c>
     </row>
     <row r="64" spans="1:47" ht="15" thickBot="1">
-      <c r="A64" t="s">
-        <v>312</v>
+      <c r="A64">
+        <v>1</v>
       </c>
       <c r="B64" t="s">
         <v>21</v>
@@ -54286,8 +54290,8 @@
       </c>
     </row>
     <row r="65" spans="1:47" ht="15" thickBot="1">
-      <c r="A65" t="s">
-        <v>292</v>
+      <c r="A65">
+        <v>1</v>
       </c>
       <c r="B65" t="s">
         <v>21</v>
@@ -54429,8 +54433,8 @@
       </c>
     </row>
     <row r="66" spans="1:47" ht="15" thickBot="1">
-      <c r="A66" t="s">
-        <v>296</v>
+      <c r="A66">
+        <v>1</v>
       </c>
       <c r="B66" t="s">
         <v>28</v>
@@ -54569,8 +54573,8 @@
       </c>
     </row>
     <row r="67" spans="1:47" ht="15" thickBot="1">
-      <c r="A67" t="s">
-        <v>288</v>
+      <c r="A67">
+        <v>1</v>
       </c>
       <c r="B67" t="s">
         <v>28</v>
@@ -54712,8 +54716,8 @@
       </c>
     </row>
     <row r="68" spans="1:47" ht="15" thickBot="1">
-      <c r="A68" t="s">
-        <v>322</v>
+      <c r="A68">
+        <v>1</v>
       </c>
       <c r="B68" t="s">
         <v>31</v>
@@ -54855,8 +54859,8 @@
       </c>
     </row>
     <row r="69" spans="1:47">
-      <c r="A69" t="s">
-        <v>570</v>
+      <c r="A69">
+        <v>1</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -54998,8 +55002,8 @@
       </c>
     </row>
     <row r="70" spans="1:47">
-      <c r="A70" t="s">
-        <v>392</v>
+      <c r="A70">
+        <v>1</v>
       </c>
       <c r="B70" t="s">
         <v>25</v>
@@ -55141,8 +55145,8 @@
       </c>
     </row>
     <row r="71" spans="1:47" ht="15" thickBot="1">
-      <c r="A71" t="s">
-        <v>345</v>
+      <c r="A71">
+        <v>1</v>
       </c>
       <c r="B71" t="s">
         <v>21</v>
@@ -55284,8 +55288,8 @@
       </c>
     </row>
     <row r="72" spans="1:47">
-      <c r="A72" t="s">
-        <v>385</v>
+      <c r="A72">
+        <v>1</v>
       </c>
       <c r="B72" t="s">
         <v>28</v>
@@ -55427,8 +55431,8 @@
       </c>
     </row>
     <row r="73" spans="1:47" ht="15" thickBot="1">
-      <c r="A73" t="s">
-        <v>620</v>
+      <c r="A73">
+        <v>1</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
@@ -55570,8 +55574,8 @@
       </c>
     </row>
     <row r="74" spans="1:47">
-      <c r="A74" t="s">
-        <v>326</v>
+      <c r="A74">
+        <v>1</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
@@ -55707,8 +55711,8 @@
       </c>
     </row>
     <row r="75" spans="1:47">
-      <c r="A75" t="s">
-        <v>560</v>
+      <c r="A75">
+        <v>1</v>
       </c>
       <c r="B75" t="s">
         <v>21</v>
@@ -55850,8 +55854,8 @@
       </c>
     </row>
     <row r="76" spans="1:47" ht="15" thickBot="1">
-      <c r="A76" t="s">
-        <v>588</v>
+      <c r="A76">
+        <v>1</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
@@ -55993,8 +55997,8 @@
       </c>
     </row>
     <row r="77" spans="1:47">
-      <c r="A77" t="s">
-        <v>647</v>
+      <c r="A77">
+        <v>1</v>
       </c>
       <c r="B77" t="s">
         <v>25</v>
@@ -56134,8 +56138,8 @@
       </c>
     </row>
     <row r="78" spans="1:47" ht="15" thickBot="1">
-      <c r="A78" t="s">
-        <v>366</v>
+      <c r="A78">
+        <v>1</v>
       </c>
       <c r="B78" t="s">
         <v>25</v>
@@ -56277,8 +56281,8 @@
       </c>
     </row>
     <row r="79" spans="1:47" ht="15" thickBot="1">
-      <c r="A79" t="s">
-        <v>513</v>
+      <c r="A79">
+        <v>1</v>
       </c>
       <c r="B79" t="s">
         <v>31</v>
@@ -56420,8 +56424,8 @@
       </c>
     </row>
     <row r="80" spans="1:47">
-      <c r="A80" t="s">
-        <v>213</v>
+      <c r="A80">
+        <v>1</v>
       </c>
       <c r="B80" t="s">
         <v>28</v>
@@ -56563,8 +56567,8 @@
       </c>
     </row>
     <row r="81" spans="1:47" ht="15" thickBot="1">
-      <c r="A81" t="s">
-        <v>93</v>
+      <c r="A81">
+        <v>1</v>
       </c>
       <c r="B81" t="s">
         <v>25</v>
@@ -56703,8 +56707,8 @@
       </c>
     </row>
     <row r="82" spans="1:47" ht="15" thickBot="1">
-      <c r="A82" t="s">
-        <v>335</v>
+      <c r="A82">
+        <v>1</v>
       </c>
       <c r="B82" t="s">
         <v>31</v>
@@ -56846,8 +56850,8 @@
       </c>
     </row>
     <row r="83" spans="1:47" ht="15" thickBot="1">
-      <c r="A83" t="s">
-        <v>460</v>
+      <c r="A83">
+        <v>1</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>
@@ -56989,8 +56993,8 @@
       </c>
     </row>
     <row r="84" spans="1:47" ht="15" thickBot="1">
-      <c r="A84" t="s">
-        <v>577</v>
+      <c r="A84">
+        <v>1</v>
       </c>
       <c r="B84" t="s">
         <v>25</v>
@@ -57132,8 +57136,8 @@
       </c>
     </row>
     <row r="85" spans="1:47" ht="15" thickBot="1">
-      <c r="A85" t="s">
-        <v>340</v>
+      <c r="A85">
+        <v>1</v>
       </c>
       <c r="B85" t="s">
         <v>36</v>
@@ -57275,8 +57279,8 @@
       </c>
     </row>
     <row r="86" spans="1:47" ht="15" thickBot="1">
-      <c r="A86" s="7" t="s">
-        <v>697</v>
+      <c r="A86">
+        <v>1</v>
       </c>
       <c r="B86" t="s">
         <v>21</v>
@@ -57418,8 +57422,8 @@
       </c>
     </row>
     <row r="87" spans="1:47">
-      <c r="A87" t="s">
-        <v>173</v>
+      <c r="A87">
+        <v>1</v>
       </c>
       <c r="B87" t="s">
         <v>36</v>
@@ -57555,8 +57559,8 @@
       </c>
     </row>
     <row r="88" spans="1:47" ht="15" thickBot="1">
-      <c r="A88" t="s">
-        <v>137</v>
+      <c r="A88">
+        <v>1</v>
       </c>
       <c r="B88" t="s">
         <v>21</v>
@@ -57698,8 +57702,8 @@
       </c>
     </row>
     <row r="89" spans="1:47" ht="15" thickBot="1">
-      <c r="A89" t="s">
-        <v>532</v>
+      <c r="A89">
+        <v>1</v>
       </c>
       <c r="B89" t="s">
         <v>31</v>
@@ -57841,8 +57845,8 @@
       </c>
     </row>
     <row r="90" spans="1:47">
-      <c r="A90" t="s">
-        <v>205</v>
+      <c r="A90">
+        <v>1</v>
       </c>
       <c r="B90" t="s">
         <v>21</v>
@@ -57984,8 +57988,8 @@
       </c>
     </row>
     <row r="91" spans="1:47">
-      <c r="A91" t="s">
-        <v>310</v>
+      <c r="A91">
+        <v>1</v>
       </c>
       <c r="B91" t="s">
         <v>31</v>
@@ -58124,8 +58128,8 @@
       </c>
     </row>
     <row r="92" spans="1:47">
-      <c r="A92" t="s">
-        <v>227</v>
+      <c r="A92">
+        <v>1</v>
       </c>
       <c r="B92" t="s">
         <v>36</v>
@@ -58267,8 +58271,8 @@
       </c>
     </row>
     <row r="93" spans="1:47" ht="15" thickBot="1">
-      <c r="A93" t="s">
-        <v>249</v>
+      <c r="A93">
+        <v>1</v>
       </c>
       <c r="B93" t="s">
         <v>21</v>
@@ -58410,8 +58414,8 @@
       </c>
     </row>
     <row r="94" spans="1:47" ht="15" thickBot="1">
-      <c r="A94" t="s">
-        <v>408</v>
+      <c r="A94">
+        <v>1</v>
       </c>
       <c r="B94" t="s">
         <v>21</v>
@@ -58544,8 +58548,8 @@
       </c>
     </row>
     <row r="95" spans="1:47">
-      <c r="A95" t="s">
-        <v>614</v>
+      <c r="A95">
+        <v>1</v>
       </c>
       <c r="B95" t="s">
         <v>21</v>
@@ -58684,8 +58688,8 @@
       </c>
     </row>
     <row r="96" spans="1:47" ht="15" thickBot="1">
-      <c r="A96" t="s">
-        <v>237</v>
+      <c r="A96">
+        <v>1</v>
       </c>
       <c r="B96" t="s">
         <v>31</v>
@@ -58827,8 +58831,8 @@
       </c>
     </row>
     <row r="97" spans="1:47" ht="15" thickBot="1">
-      <c r="A97" t="s">
-        <v>406</v>
+      <c r="A97">
+        <v>1</v>
       </c>
       <c r="B97" t="s">
         <v>31</v>
@@ -58970,8 +58974,8 @@
       </c>
     </row>
     <row r="98" spans="1:47">
-      <c r="A98" t="s">
-        <v>416</v>
+      <c r="A98">
+        <v>1</v>
       </c>
       <c r="B98" t="s">
         <v>21</v>
@@ -59113,8 +59117,8 @@
       </c>
     </row>
     <row r="99" spans="1:47" ht="15" thickBot="1">
-      <c r="A99" t="s">
-        <v>606</v>
+      <c r="A99">
+        <v>1</v>
       </c>
       <c r="B99" t="s">
         <v>31</v>
@@ -59256,8 +59260,8 @@
       </c>
     </row>
     <row r="100" spans="1:47" ht="15" thickBot="1">
-      <c r="A100" t="s">
-        <v>476</v>
+      <c r="A100">
+        <v>1</v>
       </c>
       <c r="B100" t="s">
         <v>28</v>
@@ -59399,8 +59403,8 @@
       </c>
     </row>
     <row r="101" spans="1:47">
-      <c r="A101" t="s">
-        <v>241</v>
+      <c r="A101">
+        <v>1</v>
       </c>
       <c r="B101" t="s">
         <v>36</v>
@@ -59537,8 +59541,8 @@
       </c>
     </row>
     <row r="102" spans="1:47" ht="15" thickBot="1">
-      <c r="A102" t="s">
-        <v>65</v>
+      <c r="A102">
+        <v>1</v>
       </c>
       <c r="B102" t="s">
         <v>25</v>
@@ -59680,8 +59684,8 @@
       </c>
     </row>
     <row r="103" spans="1:47">
-      <c r="A103" t="s">
-        <v>418</v>
+      <c r="A103">
+        <v>1</v>
       </c>
       <c r="B103" t="s">
         <v>21</v>
@@ -59823,8 +59827,8 @@
       </c>
     </row>
     <row r="104" spans="1:47">
-      <c r="A104" t="s">
-        <v>190</v>
+      <c r="A104">
+        <v>1</v>
       </c>
       <c r="B104" t="s">
         <v>21</v>
@@ -59966,8 +59970,8 @@
       </c>
     </row>
     <row r="105" spans="1:47" ht="15" thickBot="1">
-      <c r="A105" t="s">
-        <v>215</v>
+      <c r="A105">
+        <v>1</v>
       </c>
       <c r="B105" t="s">
         <v>21</v>
@@ -60109,8 +60113,8 @@
       </c>
     </row>
     <row r="106" spans="1:47" ht="15" thickBot="1">
-      <c r="A106" t="s">
-        <v>318</v>
+      <c r="A106">
+        <v>1</v>
       </c>
       <c r="B106" t="s">
         <v>31</v>
@@ -60252,8 +60256,8 @@
       </c>
     </row>
     <row r="107" spans="1:47" ht="15" thickBot="1">
-      <c r="A107" t="s">
-        <v>50</v>
+      <c r="A107">
+        <v>1</v>
       </c>
       <c r="B107" t="s">
         <v>28</v>
@@ -60395,8 +60399,8 @@
       </c>
     </row>
     <row r="108" spans="1:47" ht="15" thickBot="1">
-      <c r="A108" t="s">
-        <v>586</v>
+      <c r="A108">
+        <v>1</v>
       </c>
       <c r="B108" t="s">
         <v>36</v>
@@ -60527,8 +60531,8 @@
       </c>
     </row>
     <row r="109" spans="1:47" ht="15" thickBot="1">
-      <c r="A109" t="s">
-        <v>495</v>
+      <c r="A109">
+        <v>1</v>
       </c>
       <c r="B109" t="s">
         <v>25</v>
@@ -60670,8 +60674,8 @@
       </c>
     </row>
     <row r="110" spans="1:47">
-      <c r="A110" t="s">
-        <v>665</v>
+      <c r="A110">
+        <v>1</v>
       </c>
       <c r="B110" t="s">
         <v>36</v>
@@ -60811,8 +60815,8 @@
       </c>
     </row>
     <row r="111" spans="1:47" ht="15" thickBot="1">
-      <c r="A111" t="s">
-        <v>556</v>
+      <c r="A111">
+        <v>1</v>
       </c>
       <c r="B111" t="s">
         <v>28</v>
@@ -60954,8 +60958,8 @@
       </c>
     </row>
     <row r="112" spans="1:47" ht="15" thickBot="1">
-      <c r="A112" t="s">
-        <v>113</v>
+      <c r="A112">
+        <v>1</v>
       </c>
       <c r="B112" t="s">
         <v>31</v>
@@ -61097,8 +61101,8 @@
       </c>
     </row>
     <row r="113" spans="1:47" ht="15" thickBot="1">
-      <c r="A113" t="s">
-        <v>470</v>
+      <c r="A113">
+        <v>1</v>
       </c>
       <c r="B113" t="s">
         <v>31</v>
@@ -61240,8 +61244,8 @@
       </c>
     </row>
     <row r="114" spans="1:47">
-      <c r="A114" t="s">
-        <v>194</v>
+      <c r="A114">
+        <v>1</v>
       </c>
       <c r="B114" t="s">
         <v>31</v>
@@ -61383,8 +61387,8 @@
       </c>
     </row>
     <row r="115" spans="1:47">
-      <c r="A115" t="s">
-        <v>548</v>
+      <c r="A115">
+        <v>1</v>
       </c>
       <c r="B115" t="s">
         <v>25</v>
@@ -61522,8 +61526,8 @@
       </c>
     </row>
     <row r="116" spans="1:47" ht="15" thickBot="1">
-      <c r="A116" t="s">
-        <v>188</v>
+      <c r="A116">
+        <v>1</v>
       </c>
       <c r="B116" t="s">
         <v>31</v>
@@ -61665,8 +61669,8 @@
       </c>
     </row>
     <row r="117" spans="1:47" ht="15" thickBot="1">
-      <c r="A117" t="s">
-        <v>111</v>
+      <c r="A117">
+        <v>1</v>
       </c>
       <c r="B117" t="s">
         <v>28</v>
@@ -61808,8 +61812,8 @@
       </c>
     </row>
     <row r="118" spans="1:47" ht="15" thickBot="1">
-      <c r="A118" t="s">
-        <v>314</v>
+      <c r="A118">
+        <v>1</v>
       </c>
       <c r="B118" t="s">
         <v>21</v>
@@ -61951,8 +61955,8 @@
       </c>
     </row>
     <row r="119" spans="1:47" ht="15" thickBot="1">
-      <c r="A119" t="s">
-        <v>301</v>
+      <c r="A119">
+        <v>1</v>
       </c>
       <c r="B119" t="s">
         <v>31</v>
@@ -62090,8 +62094,8 @@
       </c>
     </row>
     <row r="120" spans="1:47">
-      <c r="A120" t="s">
-        <v>439</v>
+      <c r="A120">
+        <v>1</v>
       </c>
       <c r="B120" t="s">
         <v>21</v>
@@ -62233,8 +62237,8 @@
       </c>
     </row>
     <row r="121" spans="1:47" ht="15" thickBot="1">
-      <c r="A121" t="s">
-        <v>119</v>
+      <c r="A121">
+        <v>1</v>
       </c>
       <c r="B121" t="s">
         <v>31</v>
@@ -62376,8 +62380,8 @@
       </c>
     </row>
     <row r="122" spans="1:47">
-      <c r="A122" t="s">
-        <v>265</v>
+      <c r="A122">
+        <v>1</v>
       </c>
       <c r="B122" t="s">
         <v>36</v>
@@ -62519,8 +62523,8 @@
       </c>
     </row>
     <row r="123" spans="1:47">
-      <c r="A123" t="s">
-        <v>97</v>
+      <c r="A123">
+        <v>1</v>
       </c>
       <c r="B123" t="s">
         <v>28</v>
@@ -62662,8 +62666,8 @@
       </c>
     </row>
     <row r="124" spans="1:47">
-      <c r="A124" t="s">
-        <v>462</v>
+      <c r="A124">
+        <v>1</v>
       </c>
       <c r="B124" t="s">
         <v>31</v>
@@ -62805,8 +62809,8 @@
       </c>
     </row>
     <row r="125" spans="1:47" ht="15" thickBot="1">
-      <c r="A125" t="s">
-        <v>60</v>
+      <c r="A125">
+        <v>1</v>
       </c>
       <c r="B125" t="s">
         <v>28</v>
@@ -62948,8 +62952,8 @@
       </c>
     </row>
     <row r="126" spans="1:47">
-      <c r="A126" t="s">
-        <v>667</v>
+      <c r="A126">
+        <v>1</v>
       </c>
       <c r="B126" t="s">
         <v>28</v>
@@ -63091,8 +63095,8 @@
       </c>
     </row>
     <row r="127" spans="1:47" ht="15" thickBot="1">
-      <c r="A127" t="s">
-        <v>630</v>
+      <c r="A127">
+        <v>1</v>
       </c>
       <c r="B127" t="s">
         <v>31</v>
@@ -63232,8 +63236,8 @@
       </c>
     </row>
     <row r="128" spans="1:47" ht="15" thickBot="1">
-      <c r="A128" t="s">
-        <v>441</v>
+      <c r="A128">
+        <v>1</v>
       </c>
       <c r="B128" t="s">
         <v>25</v>
@@ -63375,8 +63379,8 @@
       </c>
     </row>
     <row r="129" spans="1:47">
-      <c r="A129" t="s">
-        <v>95</v>
+      <c r="A129">
+        <v>1</v>
       </c>
       <c r="B129" t="s">
         <v>28</v>
@@ -63508,8 +63512,8 @@
       </c>
     </row>
     <row r="130" spans="1:47">
-      <c r="A130" t="s">
-        <v>324</v>
+      <c r="A130">
+        <v>1</v>
       </c>
       <c r="B130" t="s">
         <v>25</v>
@@ -63648,8 +63652,8 @@
       </c>
     </row>
     <row r="131" spans="1:47" ht="15" thickBot="1">
-      <c r="A131" t="s">
-        <v>468</v>
+      <c r="A131">
+        <v>1</v>
       </c>
       <c r="B131" t="s">
         <v>25</v>
@@ -63791,8 +63795,8 @@
       </c>
     </row>
     <row r="132" spans="1:47">
-      <c r="A132" t="s">
-        <v>628</v>
+      <c r="A132">
+        <v>1</v>
       </c>
       <c r="B132" t="s">
         <v>21</v>
@@ -63934,8 +63938,8 @@
       </c>
     </row>
     <row r="133" spans="1:47">
-      <c r="A133" t="s">
-        <v>67</v>
+      <c r="A133">
+        <v>1</v>
       </c>
       <c r="B133" t="s">
         <v>25</v>
@@ -64075,8 +64079,8 @@
       </c>
     </row>
     <row r="134" spans="1:47" ht="15" thickBot="1">
-      <c r="A134" t="s">
-        <v>426</v>
+      <c r="A134">
+        <v>1</v>
       </c>
       <c r="B134" t="s">
         <v>28</v>
@@ -64218,8 +64222,8 @@
       </c>
     </row>
     <row r="135" spans="1:47">
-      <c r="A135" t="s">
-        <v>660</v>
+      <c r="A135">
+        <v>1</v>
       </c>
       <c r="B135" t="s">
         <v>21</v>
@@ -64351,8 +64355,8 @@
       </c>
     </row>
     <row r="136" spans="1:47">
-      <c r="A136" t="s">
-        <v>259</v>
+      <c r="A136">
+        <v>1</v>
       </c>
       <c r="B136" t="s">
         <v>21</v>
@@ -64494,8 +64498,8 @@
       </c>
     </row>
     <row r="137" spans="1:47" ht="15" thickBot="1">
-      <c r="A137" t="s">
-        <v>38</v>
+      <c r="A137">
+        <v>1</v>
       </c>
       <c r="B137" t="s">
         <v>21</v>
@@ -64637,8 +64641,8 @@
       </c>
     </row>
     <row r="138" spans="1:47" ht="15" thickBot="1">
-      <c r="A138" t="s">
-        <v>564</v>
+      <c r="A138">
+        <v>1</v>
       </c>
       <c r="B138" t="s">
         <v>31</v>
@@ -64778,8 +64782,8 @@
       </c>
     </row>
     <row r="139" spans="1:47" ht="15" thickBot="1">
-      <c r="A139" t="s">
-        <v>445</v>
+      <c r="A139">
+        <v>1</v>
       </c>
       <c r="B139" t="s">
         <v>31</v>
@@ -64921,8 +64925,8 @@
       </c>
     </row>
     <row r="140" spans="1:47">
-      <c r="A140" t="s">
-        <v>219</v>
+      <c r="A140">
+        <v>1</v>
       </c>
       <c r="B140" t="s">
         <v>21</v>
@@ -65049,8 +65053,8 @@
       </c>
     </row>
     <row r="141" spans="1:47">
-      <c r="A141" t="s">
-        <v>566</v>
+      <c r="A141">
+        <v>1</v>
       </c>
       <c r="B141" t="s">
         <v>25</v>
@@ -65192,8 +65196,8 @@
       </c>
     </row>
     <row r="142" spans="1:47" ht="15" thickBot="1">
-      <c r="A142" t="s">
-        <v>258</v>
+      <c r="A142">
+        <v>1</v>
       </c>
       <c r="B142" t="s">
         <v>21</v>
@@ -65333,8 +65337,8 @@
       </c>
     </row>
     <row r="143" spans="1:47" ht="15" thickBot="1">
-      <c r="A143" t="s">
-        <v>651</v>
+      <c r="A143">
+        <v>1</v>
       </c>
       <c r="B143" t="s">
         <v>21</v>
@@ -65476,8 +65480,8 @@
       </c>
     </row>
     <row r="144" spans="1:47">
-      <c r="A144" t="s">
-        <v>491</v>
+      <c r="A144">
+        <v>1</v>
       </c>
       <c r="B144" t="s">
         <v>21</v>
@@ -65619,8 +65623,8 @@
       </c>
     </row>
     <row r="145" spans="1:47">
-      <c r="A145" t="s">
-        <v>262</v>
+      <c r="A145">
+        <v>1</v>
       </c>
       <c r="B145" t="s">
         <v>31</v>
@@ -65762,8 +65766,8 @@
       </c>
     </row>
     <row r="146" spans="1:47" ht="15" thickBot="1">
-      <c r="A146" t="s">
-        <v>485</v>
+      <c r="A146">
+        <v>1</v>
       </c>
       <c r="B146" t="s">
         <v>21</v>
@@ -65903,8 +65907,8 @@
       </c>
     </row>
     <row r="147" spans="1:47" ht="15" thickBot="1">
-      <c r="A147" t="s">
-        <v>633</v>
+      <c r="A147">
+        <v>1</v>
       </c>
       <c r="B147" t="s">
         <v>36</v>
@@ -66046,8 +66050,8 @@
       </c>
     </row>
     <row r="148" spans="1:47" ht="15" thickBot="1">
-      <c r="A148" t="s">
-        <v>279</v>
+      <c r="A148">
+        <v>1</v>
       </c>
       <c r="B148" t="s">
         <v>25</v>
@@ -66189,8 +66193,8 @@
       </c>
     </row>
     <row r="149" spans="1:47" ht="15" thickBot="1">
-      <c r="A149" t="s">
-        <v>353</v>
+      <c r="A149">
+        <v>1</v>
       </c>
       <c r="B149" t="s">
         <v>28</v>
@@ -66322,8 +66326,8 @@
       </c>
     </row>
     <row r="150" spans="1:47" ht="15" thickBot="1">
-      <c r="A150" t="s">
-        <v>77</v>
+      <c r="A150">
+        <v>1</v>
       </c>
       <c r="B150" t="s">
         <v>28</v>
@@ -66465,8 +66469,8 @@
       </c>
     </row>
     <row r="151" spans="1:47" ht="15" thickBot="1">
-      <c r="A151" t="s">
-        <v>85</v>
+      <c r="A151">
+        <v>1</v>
       </c>
       <c r="B151" t="s">
         <v>36</v>
@@ -66598,8 +66602,8 @@
       </c>
     </row>
     <row r="152" spans="1:47" ht="15" thickBot="1">
-      <c r="A152" t="s">
-        <v>89</v>
+      <c r="A152">
+        <v>1</v>
       </c>
       <c r="B152" t="s">
         <v>28</v>
@@ -66739,8 +66743,8 @@
       </c>
     </row>
     <row r="153" spans="1:47" ht="15" thickBot="1">
-      <c r="A153" t="s">
-        <v>91</v>
+      <c r="A153">
+        <v>1</v>
       </c>
       <c r="B153" t="s">
         <v>21</v>
@@ -66882,8 +66886,8 @@
       </c>
     </row>
     <row r="154" spans="1:47" ht="15" thickBot="1">
-      <c r="A154" t="s">
-        <v>107</v>
+      <c r="A154">
+        <v>1</v>
       </c>
       <c r="B154" t="s">
         <v>28</v>
@@ -67025,8 +67029,8 @@
       </c>
     </row>
     <row r="155" spans="1:47" ht="15" thickBot="1">
-      <c r="A155" t="s">
-        <v>151</v>
+      <c r="A155">
+        <v>1</v>
       </c>
       <c r="B155" t="s">
         <v>25</v>
@@ -67166,8 +67170,8 @@
       </c>
     </row>
     <row r="156" spans="1:47" ht="15" thickBot="1">
-      <c r="A156" t="s">
-        <v>157</v>
+      <c r="A156">
+        <v>1</v>
       </c>
       <c r="B156" t="s">
         <v>21</v>
@@ -67309,8 +67313,8 @@
       </c>
     </row>
     <row r="157" spans="1:47" ht="15" thickBot="1">
-      <c r="A157" t="s">
-        <v>159</v>
+      <c r="A157">
+        <v>1</v>
       </c>
       <c r="B157" t="s">
         <v>31</v>
@@ -67452,8 +67456,8 @@
       </c>
     </row>
     <row r="158" spans="1:47" ht="15" thickBot="1">
-      <c r="A158" t="s">
-        <v>179</v>
+      <c r="A158">
+        <v>1</v>
       </c>
       <c r="B158" t="s">
         <v>31</v>
@@ -67595,8 +67599,8 @@
       </c>
     </row>
     <row r="159" spans="1:47" ht="15" thickBot="1">
-      <c r="A159" t="s">
-        <v>261</v>
+      <c r="A159">
+        <v>1</v>
       </c>
       <c r="B159" t="s">
         <v>36</v>
@@ -67736,8 +67740,8 @@
       </c>
     </row>
     <row r="160" spans="1:47">
-      <c r="A160" t="s">
-        <v>273</v>
+      <c r="A160">
+        <v>1</v>
       </c>
       <c r="B160" t="s">
         <v>21</v>
@@ -67877,8 +67881,8 @@
       </c>
     </row>
     <row r="161" spans="1:47">
-      <c r="A161" t="s">
-        <v>320</v>
+      <c r="A161">
+        <v>1</v>
       </c>
       <c r="B161" t="s">
         <v>31</v>
@@ -68018,8 +68022,8 @@
       </c>
     </row>
     <row r="162" spans="1:47" ht="15" thickBot="1">
-      <c r="A162" t="s">
-        <v>354</v>
+      <c r="A162">
+        <v>1</v>
       </c>
       <c r="B162" t="s">
         <v>31</v>
@@ -68161,8 +68165,8 @@
       </c>
     </row>
     <row r="163" spans="1:47" ht="15" thickBot="1">
-      <c r="A163" t="s">
-        <v>363</v>
+      <c r="A163">
+        <v>1</v>
       </c>
       <c r="B163" t="s">
         <v>31</v>
@@ -68304,8 +68308,8 @@
       </c>
     </row>
     <row r="164" spans="1:47">
-      <c r="A164" t="s">
-        <v>374</v>
+      <c r="A164">
+        <v>1</v>
       </c>
       <c r="B164" t="s">
         <v>31</v>
@@ -68444,8 +68448,8 @@
       </c>
     </row>
     <row r="165" spans="1:47" ht="15" thickBot="1">
-      <c r="A165" t="s">
-        <v>404</v>
+      <c r="A165">
+        <v>1</v>
       </c>
       <c r="B165" t="s">
         <v>28</v>
@@ -68587,8 +68591,8 @@
       </c>
     </row>
     <row r="166" spans="1:47" ht="15" thickBot="1">
-      <c r="A166" t="s">
-        <v>410</v>
+      <c r="A166">
+        <v>1</v>
       </c>
       <c r="B166" t="s">
         <v>31</v>
@@ -68730,8 +68734,8 @@
       </c>
     </row>
     <row r="167" spans="1:47" ht="15" thickBot="1">
-      <c r="A167" t="s">
-        <v>511</v>
+      <c r="A167">
+        <v>1</v>
       </c>
       <c r="B167" t="s">
         <v>21</v>
@@ -68873,8 +68877,8 @@
       </c>
     </row>
     <row r="168" spans="1:47" ht="15" thickBot="1">
-      <c r="A168" t="s">
-        <v>528</v>
+      <c r="A168">
+        <v>1</v>
       </c>
       <c r="B168" t="s">
         <v>31</v>
@@ -69012,8 +69016,8 @@
       </c>
     </row>
     <row r="169" spans="1:47">
-      <c r="A169" t="s">
-        <v>547</v>
+      <c r="A169">
+        <v>1</v>
       </c>
       <c r="B169" t="s">
         <v>21</v>
@@ -69153,8 +69157,8 @@
       </c>
     </row>
     <row r="170" spans="1:47">
-      <c r="A170" t="s">
-        <v>20</v>
+      <c r="A170">
+        <v>1</v>
       </c>
       <c r="B170" t="s">
         <v>21</v>
@@ -69296,8 +69300,8 @@
       </c>
     </row>
     <row r="171" spans="1:47" ht="15" thickBot="1">
-      <c r="A171" t="s">
-        <v>27</v>
+      <c r="A171">
+        <v>1</v>
       </c>
       <c r="B171" t="s">
         <v>28</v>
@@ -69439,8 +69443,8 @@
       </c>
     </row>
     <row r="172" spans="1:47" ht="15" thickBot="1">
-      <c r="A172" t="s">
-        <v>30</v>
+      <c r="A172">
+        <v>1</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
@@ -69582,8 +69586,8 @@
       </c>
     </row>
     <row r="173" spans="1:47" ht="15" thickBot="1">
-      <c r="A173" t="s">
-        <v>153</v>
+      <c r="A173">
+        <v>1</v>
       </c>
       <c r="B173" t="s">
         <v>25</v>
@@ -69722,8 +69726,8 @@
       </c>
     </row>
     <row r="174" spans="1:47" ht="15" thickBot="1">
-      <c r="A174" t="s">
-        <v>162</v>
+      <c r="A174">
+        <v>1</v>
       </c>
       <c r="B174" t="s">
         <v>28</v>
@@ -69865,8 +69869,8 @@
       </c>
     </row>
     <row r="175" spans="1:47">
-      <c r="A175" t="s">
-        <v>184</v>
+      <c r="A175">
+        <v>1</v>
       </c>
       <c r="B175" t="s">
         <v>25</v>
@@ -70008,8 +70012,8 @@
       </c>
     </row>
     <row r="176" spans="1:47">
-      <c r="A176" t="s">
-        <v>239</v>
+      <c r="A176">
+        <v>1</v>
       </c>
       <c r="B176" t="s">
         <v>28</v>
@@ -70151,8 +70155,8 @@
       </c>
     </row>
     <row r="177" spans="1:47" ht="15" thickBot="1">
-      <c r="A177" t="s">
-        <v>253</v>
+      <c r="A177">
+        <v>1</v>
       </c>
       <c r="B177" t="s">
         <v>28</v>
@@ -70290,8 +70294,8 @@
       </c>
     </row>
     <row r="178" spans="1:47">
-      <c r="A178" t="s">
-        <v>466</v>
+      <c r="A178">
+        <v>1</v>
       </c>
       <c r="B178" t="s">
         <v>21</v>
@@ -70433,8 +70437,8 @@
       </c>
     </row>
     <row r="179" spans="1:47" ht="15" thickBot="1">
-      <c r="A179" t="s">
-        <v>542</v>
+      <c r="A179">
+        <v>1</v>
       </c>
       <c r="B179" t="s">
         <v>28</v>
@@ -70576,8 +70580,8 @@
       </c>
     </row>
     <row r="180" spans="1:47" ht="15" thickBot="1">
-      <c r="A180" t="s">
-        <v>608</v>
+      <c r="A180">
+        <v>1</v>
       </c>
       <c r="B180" t="s">
         <v>31</v>
@@ -70719,8 +70723,8 @@
       </c>
     </row>
     <row r="181" spans="1:47">
-      <c r="A181" t="s">
-        <v>627</v>
+      <c r="A181">
+        <v>1</v>
       </c>
       <c r="B181" t="s">
         <v>28</v>
@@ -70862,8 +70866,8 @@
       </c>
     </row>
     <row r="182" spans="1:47" ht="15" thickBot="1">
-      <c r="A182" t="s">
-        <v>644</v>
+      <c r="A182">
+        <v>1</v>
       </c>
       <c r="B182" t="s">
         <v>25</v>
@@ -70999,8 +71003,8 @@
       </c>
     </row>
     <row r="183" spans="1:47" ht="15" thickBot="1">
-      <c r="A183" t="s">
-        <v>645</v>
+      <c r="A183">
+        <v>1</v>
       </c>
       <c r="B183" t="s">
         <v>31</v>
@@ -71142,8 +71146,8 @@
       </c>
     </row>
     <row r="184" spans="1:47">
-      <c r="A184" t="s">
-        <v>48</v>
+      <c r="A184">
+        <v>1</v>
       </c>
       <c r="B184" t="s">
         <v>31</v>
@@ -71282,8 +71286,8 @@
       </c>
     </row>
     <row r="185" spans="1:47">
-      <c r="A185" t="s">
-        <v>105</v>
+      <c r="A185">
+        <v>1</v>
       </c>
       <c r="B185" t="s">
         <v>21</v>
@@ -71419,8 +71423,8 @@
       </c>
     </row>
     <row r="186" spans="1:47" ht="15" thickBot="1">
-      <c r="A186" t="s">
-        <v>125</v>
+      <c r="A186">
+        <v>1</v>
       </c>
       <c r="B186" t="s">
         <v>28</v>
@@ -71559,8 +71563,8 @@
       </c>
     </row>
     <row r="187" spans="1:47">
-      <c r="A187" t="s">
-        <v>147</v>
+      <c r="A187">
+        <v>1</v>
       </c>
       <c r="B187" t="s">
         <v>21</v>
@@ -71700,8 +71704,8 @@
       </c>
     </row>
     <row r="188" spans="1:47" ht="15" thickBot="1">
-      <c r="A188" t="s">
-        <v>149</v>
+      <c r="A188">
+        <v>1</v>
       </c>
       <c r="B188" t="s">
         <v>25</v>
@@ -71843,8 +71847,8 @@
       </c>
     </row>
     <row r="189" spans="1:47">
-      <c r="A189" t="s">
-        <v>164</v>
+      <c r="A189">
+        <v>1</v>
       </c>
       <c r="B189" t="s">
         <v>31</v>
@@ -71986,8 +71990,8 @@
       </c>
     </row>
     <row r="190" spans="1:47" ht="15" thickBot="1">
-      <c r="A190" t="s">
-        <v>198</v>
+      <c r="A190">
+        <v>1</v>
       </c>
       <c r="B190" t="s">
         <v>21</v>
@@ -72129,8 +72133,8 @@
       </c>
     </row>
     <row r="191" spans="1:47">
-      <c r="A191" t="s">
-        <v>200</v>
+      <c r="A191">
+        <v>1</v>
       </c>
       <c r="B191" t="s">
         <v>21</v>
@@ -72272,8 +72276,8 @@
       </c>
     </row>
     <row r="192" spans="1:47" ht="15" thickBot="1">
-      <c r="A192" t="s">
-        <v>284</v>
+      <c r="A192">
+        <v>1</v>
       </c>
       <c r="B192" t="s">
         <v>25</v>
@@ -72415,8 +72419,8 @@
       </c>
     </row>
     <row r="193" spans="1:47" ht="15" thickBot="1">
-      <c r="A193" t="s">
-        <v>319</v>
+      <c r="A193">
+        <v>1</v>
       </c>
       <c r="B193" t="s">
         <v>25</v>
@@ -72556,8 +72560,8 @@
       </c>
     </row>
     <row r="194" spans="1:47" ht="15" thickBot="1">
-      <c r="A194" t="s">
-        <v>425</v>
+      <c r="A194">
+        <v>1</v>
       </c>
       <c r="B194" t="s">
         <v>28</v>
@@ -72697,8 +72701,8 @@
       </c>
     </row>
     <row r="195" spans="1:47" ht="15" thickBot="1">
-      <c r="A195" t="s">
-        <v>503</v>
+      <c r="A195">
+        <v>1</v>
       </c>
       <c r="B195" t="s">
         <v>21</v>
@@ -72840,8 +72844,8 @@
       </c>
     </row>
     <row r="196" spans="1:47">
-      <c r="A196" t="s">
-        <v>540</v>
+      <c r="A196">
+        <v>1</v>
       </c>
       <c r="B196" t="s">
         <v>28</v>
@@ -72983,8 +72987,8 @@
       </c>
     </row>
     <row r="197" spans="1:47">
-      <c r="A197" t="s">
-        <v>568</v>
+      <c r="A197">
+        <v>1</v>
       </c>
       <c r="B197" t="s">
         <v>21</v>
@@ -73117,8 +73121,8 @@
       </c>
     </row>
     <row r="198" spans="1:47" ht="15" thickBot="1">
-      <c r="A198" t="s">
-        <v>625</v>
+      <c r="A198">
+        <v>1</v>
       </c>
       <c r="B198" t="s">
         <v>21</v>
@@ -73260,8 +73264,8 @@
       </c>
     </row>
     <row r="199" spans="1:47" ht="15" thickBot="1">
-      <c r="A199" t="s">
-        <v>635</v>
+      <c r="A199">
+        <v>1</v>
       </c>
       <c r="B199" t="s">
         <v>31</v>
@@ -73403,8 +73407,8 @@
       </c>
     </row>
     <row r="200" spans="1:47" ht="15" thickBot="1">
-      <c r="A200" t="s">
-        <v>640</v>
+      <c r="A200">
+        <v>1</v>
       </c>
       <c r="B200" t="s">
         <v>25</v>
@@ -73525,8 +73529,8 @@
       </c>
     </row>
     <row r="201" spans="1:47" ht="15" thickBot="1">
-      <c r="A201" t="s">
-        <v>46</v>
+      <c r="A201">
+        <v>1</v>
       </c>
       <c r="B201" t="s">
         <v>21</v>
@@ -73668,8 +73672,8 @@
       </c>
     </row>
     <row r="202" spans="1:47" ht="15" thickBot="1">
-      <c r="A202" t="s">
-        <v>143</v>
+      <c r="A202">
+        <v>1</v>
       </c>
       <c r="B202" t="s">
         <v>21</v>
@@ -73811,8 +73815,8 @@
       </c>
     </row>
     <row r="203" spans="1:47">
-      <c r="A203" t="s">
-        <v>231</v>
+      <c r="A203">
+        <v>1</v>
       </c>
       <c r="B203" t="s">
         <v>21</v>
@@ -73954,8 +73958,8 @@
       </c>
     </row>
     <row r="204" spans="1:47">
-      <c r="A204" t="s">
-        <v>302</v>
+      <c r="A204">
+        <v>1</v>
       </c>
       <c r="B204" t="s">
         <v>31</v>
@@ -74097,8 +74101,8 @@
       </c>
     </row>
     <row r="205" spans="1:47" ht="15" thickBot="1">
-      <c r="A205" t="s">
-        <v>341</v>
+      <c r="A205">
+        <v>1</v>
       </c>
       <c r="B205" t="s">
         <v>31</v>
@@ -74240,8 +74244,8 @@
       </c>
     </row>
     <row r="206" spans="1:47" ht="15" thickBot="1">
-      <c r="A206" t="s">
-        <v>343</v>
+      <c r="A206">
+        <v>1</v>
       </c>
       <c r="B206" t="s">
         <v>28</v>
@@ -74380,8 +74384,8 @@
       </c>
     </row>
     <row r="207" spans="1:47" ht="15" thickBot="1">
-      <c r="A207" t="s">
-        <v>389</v>
+      <c r="A207">
+        <v>1</v>
       </c>
       <c r="B207" t="s">
         <v>21</v>
@@ -74517,8 +74521,8 @@
       </c>
     </row>
     <row r="208" spans="1:47" ht="15" thickBot="1">
-      <c r="A208" t="s">
-        <v>420</v>
+      <c r="A208">
+        <v>1</v>
       </c>
       <c r="B208" t="s">
         <v>31</v>
@@ -74657,8 +74661,8 @@
       </c>
     </row>
     <row r="209" spans="1:47">
-      <c r="A209" t="s">
-        <v>472</v>
+      <c r="A209">
+        <v>1</v>
       </c>
       <c r="B209" t="s">
         <v>28</v>
@@ -74794,8 +74798,8 @@
       </c>
     </row>
     <row r="210" spans="1:47" ht="15" thickBot="1">
-      <c r="A210" t="s">
-        <v>499</v>
+      <c r="A210">
+        <v>1</v>
       </c>
       <c r="B210" t="s">
         <v>21</v>
@@ -74937,8 +74941,8 @@
       </c>
     </row>
     <row r="211" spans="1:47" ht="15" thickBot="1">
-      <c r="A211" t="s">
-        <v>590</v>
+      <c r="A211">
+        <v>1</v>
       </c>
       <c r="B211" t="s">
         <v>21</v>
@@ -75080,8 +75084,8 @@
       </c>
     </row>
     <row r="212" spans="1:47" ht="15" thickBot="1">
-      <c r="A212" t="s">
-        <v>653</v>
+      <c r="A212">
+        <v>1</v>
       </c>
       <c r="B212" t="s">
         <v>25</v>
@@ -75223,8 +75227,8 @@
       </c>
     </row>
     <row r="213" spans="1:47">
-      <c r="A213" t="s">
-        <v>307</v>
+      <c r="A213">
+        <v>1</v>
       </c>
       <c r="B213" t="s">
         <v>28</v>
@@ -75359,8 +75363,8 @@
       </c>
     </row>
     <row r="214" spans="1:47">
-      <c r="A214" t="s">
-        <v>422</v>
+      <c r="A214">
+        <v>1</v>
       </c>
       <c r="B214" t="s">
         <v>22</v>
@@ -75502,8 +75506,8 @@
       </c>
     </row>
     <row r="215" spans="1:47" ht="15" thickBot="1">
-      <c r="A215" t="s">
-        <v>435</v>
+      <c r="A215">
+        <v>1</v>
       </c>
       <c r="B215" t="s">
         <v>28</v>
@@ -75645,8 +75649,8 @@
       </c>
     </row>
     <row r="216" spans="1:47" ht="15" thickBot="1">
-      <c r="A216" t="s">
-        <v>221</v>
+      <c r="A216">
+        <v>1</v>
       </c>
       <c r="B216" t="s">
         <v>36</v>
@@ -75788,8 +75792,8 @@
       </c>
     </row>
     <row r="217" spans="1:47">
-      <c r="A217" t="s">
-        <v>652</v>
+      <c r="A217">
+        <v>1</v>
       </c>
       <c r="B217" t="s">
         <v>28</v>
@@ -75928,8 +75932,8 @@
       </c>
     </row>
     <row r="218" spans="1:47" ht="15" thickBot="1">
-      <c r="A218" t="s">
-        <v>433</v>
+      <c r="A218">
+        <v>1</v>
       </c>
       <c r="B218" t="s">
         <v>31</v>
@@ -76065,8 +76069,8 @@
       </c>
     </row>
     <row r="219" spans="1:47" ht="15" thickBot="1">
-      <c r="A219" t="s">
-        <v>575</v>
+      <c r="A219">
+        <v>1</v>
       </c>
       <c r="B219" t="s">
         <v>25</v>
@@ -76208,8 +76212,8 @@
       </c>
     </row>
     <row r="220" spans="1:47">
-      <c r="A220" t="s">
-        <v>329</v>
+      <c r="A220">
+        <v>1</v>
       </c>
       <c r="B220" t="s">
         <v>31</v>
@@ -76351,8 +76355,8 @@
       </c>
     </row>
     <row r="221" spans="1:47" ht="15" thickBot="1">
-      <c r="A221" t="s">
-        <v>294</v>
+      <c r="A221">
+        <v>1</v>
       </c>
       <c r="B221" t="s">
         <v>31</v>
@@ -76494,8 +76498,8 @@
       </c>
     </row>
     <row r="222" spans="1:47">
-      <c r="A222" t="s">
-        <v>390</v>
+      <c r="A222">
+        <v>1</v>
       </c>
       <c r="B222" t="s">
         <v>21</v>
@@ -76637,10 +76641,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:FA228">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:FA228">
     <sortCondition ref="D2:D228"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -87869,6 +87874,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -98313,5 +98319,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>